<commit_message>
moose aerial general is done
</commit_message>
<xml_diff>
--- a/sims/src/observations/moose/aerial-general-recruitment-composition-survey/2.1/test-data/Moose_Aerial_General_Recruit_Comp_Survey_2.0_Test_Data.xlsx
+++ b/sims/src/observations/moose/aerial-general-recruitment-composition-survey/2.1/test-data/Moose_Aerial_General_Recruit_Comp_Survey_2.0_Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/DevelopmentProjects/biohubbc-utils/sims/src/observations/moose/aerial-general-recruitment-composition-survey/2.1/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23592C6F-2BB8-5B42-9155-280E741A487E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09849B0B-AEE0-3140-8D0B-5293467B0D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16100" tabRatio="812" activeTab="4" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
+    <workbookView xWindow="800" yWindow="520" windowWidth="25380" windowHeight="16100" tabRatio="812" activeTab="3" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Strata Metadata" sheetId="11" state="hidden" r:id="rId1"/>
@@ -1332,19 +1332,38 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-A unique identification label assigned to track a group of animals detected during the course of a Block Visit, e.g., G25, 1, etc. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A unique identification label assigned to track a group of animals detected during the course of a Block Visit, e.g., G25, 1, etc. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
             <u/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1353,13 +1372,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-INSTRUCTIONS: Labels should contain letters or number but should start with a character other than zero, and contain no hyphens. For example, 'AM330' or 'D30' will work well with Excel.
-Avoid Labels that do not contain letters, begin with zero, or contain hyphens. For example, avoid '003' or '2-5', because Excel may automatically reformat such data</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">INSTRUCTIONS: Labels should contain letters or number but should start with a character other than zero, and contain no hyphens. For example, 'AM330' or 'D30' will work well with Excel.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Avoid Labels that do not contain letters, begin with zero, or contain hyphens. For example, avoid '003' or '2-5', because Excel may automatically reformat such data</t>
         </r>
       </text>
     </comment>
@@ -1384,12 +1441,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Was this marked animal located because it was targeted, e.g. searched for using telemetry equipment, or was it located 'blindly' without the intial aid of equipment, non-targeted; Picklist</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Was this marked animal located because it was targeted, e.g. searched for using telemetry equipment, or was it located 'blindly' without the intial aid of equipment, non-targeted; Picklist</t>
         </r>
       </text>
     </comment>
@@ -1398,19 +1464,48 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-An ID provided by the Wildlife Health office which uniquely identifies an animal for the purposes of tracking its health, e.g. 22-00001; Text field
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">An ID provided by the Wildlife Health office which uniquely identifies an animal for the purposes of tracking its health, e.g. 22-00001; Text field
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
             <u/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1555,14 +1650,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-An idenifier on the left ear tag that the biologist uses to help identify the animal. Text.
-INSTRUCTIONS:
-AVOID '003' or '2-5', because data systems (e.g. Excel) often automatically reformat such data.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">An idenifier on the left ear tag that the biologist uses to help identify the animal. Text.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">INSTRUCTIONS:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AVOID '003' or '2-5', because data systems (e.g. Excel) often automatically reformat such data.</t>
         </r>
       </text>
     </comment>
@@ -13566,8 +13698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DA42AB-89CB-4281-9E1C-AE4075D8E1F6}">
   <dimension ref="A1:AQ501"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AP10" sqref="AP10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18289,9 +18421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0A6F2E-B8CC-4183-A628-4B8F278F1739}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>